<commit_message>
PCA & GPU for new sim, Stairs, and hydrant adjustments
</commit_message>
<xml_diff>
--- a/assets/Meshes/Mesh_Inspection.xlsx
+++ b/assets/Meshes/Mesh_Inspection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\assets\Meshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CFF20A-DD5C-4740-9E83-72A7941F51E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231967C8-42AB-46A8-AD8E-9B6402305FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,8 +351,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="DB109" sqref="DB109"/>
+    <sheetView tabSelected="1" topLeftCell="BN42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="DP54" sqref="DP54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21495,19 +21495,19 @@
         <v>0</v>
       </c>
       <c r="DE37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ37" s="1">
         <v>1</v>
@@ -22070,22 +22070,22 @@
         <v>0</v>
       </c>
       <c r="DD38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ38" s="1">
         <v>1</v>
@@ -22645,25 +22645,25 @@
         <v>0</v>
       </c>
       <c r="DC39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ39" s="1">
         <v>1</v>
@@ -23220,28 +23220,28 @@
         <v>0</v>
       </c>
       <c r="DB40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ40" s="1">
         <v>1</v>
@@ -23798,28 +23798,28 @@
         <v>0</v>
       </c>
       <c r="DB41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ41" s="1">
         <v>1</v>
@@ -24376,28 +24376,28 @@
         <v>0</v>
       </c>
       <c r="DB42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ42" s="1">
         <v>1</v>
@@ -24954,28 +24954,28 @@
         <v>0</v>
       </c>
       <c r="DB43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ43" s="1">
         <v>1</v>
@@ -25532,28 +25532,28 @@
         <v>0</v>
       </c>
       <c r="DB44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ44" s="1">
         <v>1</v>
@@ -26110,28 +26110,28 @@
         <v>0</v>
       </c>
       <c r="DB45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ45" s="1">
         <v>1</v>
@@ -26688,28 +26688,28 @@
         <v>0</v>
       </c>
       <c r="DB46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ46" s="1">
         <v>1</v>
@@ -27266,28 +27266,28 @@
         <v>0</v>
       </c>
       <c r="DB47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ47" s="1">
         <v>1</v>
@@ -27844,28 +27844,28 @@
         <v>0</v>
       </c>
       <c r="DB48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ48" s="1">
         <v>1</v>
@@ -28422,28 +28422,28 @@
         <v>0</v>
       </c>
       <c r="DB49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ49" s="1">
         <v>1</v>
@@ -29000,28 +29000,28 @@
         <v>0</v>
       </c>
       <c r="DB50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ50" s="1">
         <v>1</v>
@@ -29578,28 +29578,28 @@
         <v>0</v>
       </c>
       <c r="DB51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ51" s="1">
         <v>1</v>
@@ -30156,28 +30156,28 @@
         <v>0</v>
       </c>
       <c r="DB52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ52" s="1">
         <v>1</v>
@@ -30734,28 +30734,28 @@
         <v>0</v>
       </c>
       <c r="DB53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ53" s="1">
         <v>1</v>
@@ -54432,7 +54432,7 @@
         <v>0</v>
       </c>
       <c r="DB94" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC94" s="1">
         <v>1</v>
@@ -55010,13 +55010,13 @@
         <v>0</v>
       </c>
       <c r="DB95" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC95" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD95" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE95" s="1">
         <v>1</v>
@@ -55588,31 +55588,31 @@
         <v>0</v>
       </c>
       <c r="DB96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK96" s="1">
         <v>1</v>
@@ -55642,43 +55642,43 @@
         <v>1</v>
       </c>
       <c r="DT96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG96" s="1">
         <v>1</v>
@@ -56175,88 +56175,88 @@
         <v>1</v>
       </c>
       <c r="DE97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DL97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DM97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DN97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DO97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DP97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DQ97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DR97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DS97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DT97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG97" s="1">
         <v>1</v>
@@ -56759,82 +56759,82 @@
         <v>1</v>
       </c>
       <c r="DG98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DL98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DM98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DN98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DO98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DP98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DQ98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DR98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DS98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DT98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG98" s="1">
         <v>1</v>
@@ -57376,43 +57376,43 @@
         <v>1</v>
       </c>
       <c r="DT99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG99" s="1">
         <v>1</v>
@@ -57954,43 +57954,43 @@
         <v>1</v>
       </c>
       <c r="DT100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG100" s="1">
         <v>1</v>
@@ -58532,43 +58532,43 @@
         <v>1</v>
       </c>
       <c r="DT101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG101" s="1">
         <v>1</v>
@@ -59110,43 +59110,43 @@
         <v>1</v>
       </c>
       <c r="DT102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DV102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DW102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DY102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DZ102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EB102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EC102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ED102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG102" s="1">
         <v>1</v>
@@ -69400,13 +69400,13 @@
         <v>1</v>
       </c>
       <c r="CH120" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI120" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ120" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK120" s="1">
         <v>0</v>
@@ -69978,16 +69978,16 @@
         <v>1</v>
       </c>
       <c r="CH121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL121" s="1">
         <v>0</v>
@@ -70556,16 +70556,16 @@
         <v>1</v>
       </c>
       <c r="CH122" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI122" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ122" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK122" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL122" s="1">
         <v>0</v>
@@ -71134,19 +71134,19 @@
         <v>1</v>
       </c>
       <c r="CH123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM123" s="1">
         <v>0</v>
@@ -71712,19 +71712,19 @@
         <v>1</v>
       </c>
       <c r="CH124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM124" s="1">
         <v>0</v>
@@ -91686,7 +91686,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DB97:GJ126 DA115:DA126 A122:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 A116:CZ121 CJ97:DA99 A1:GJ91 A92:BY99 CJ93:GJ96 BZ93:CI99 BZ92:GJ92 A100:DA112">
+  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A92:BY99 BZ93:CI99 BZ92:GJ92 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:GJ95 DB103:GJ126 CJ96:EF96 DB97:EF102 EG96:GJ102 A1:GJ91">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -91698,7 +91698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DB97:XFD126 DA115:DA126 A122:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 A116:CZ121 CJ97:DA99 A1:XFD91 A92:BY99 CJ93:XFD96 BZ93:CI99 BZ92:XFD92 A100:DA112">
+  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A92:BY99 BZ93:CI99 BZ92:XFD92 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:XFD95 DB103:XFD126 CJ96:EF96 DB97:EF102 EG96:XFD102 A1:XFD91">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
reversing out function improved and changed
</commit_message>
<xml_diff>
--- a/assets/Meshes/Mesh_Inspection.xlsx
+++ b/assets/Meshes/Mesh_Inspection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\assets\Meshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AC2C8E-0279-4CD8-AEB6-A4C462F5C3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D84257-CE61-48BF-BA5F-7D20F7F04049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,8 +351,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="DV17" sqref="DV17"/>
+    <sheetView tabSelected="1" topLeftCell="AO61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CE93" sqref="CE93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31312,28 +31312,28 @@
         <v>0</v>
       </c>
       <c r="DB54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ54" s="1">
         <v>1</v>
@@ -48538,28 +48538,28 @@
         <v>1</v>
       </c>
       <c r="BP84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX84" s="1">
         <v>1</v>
@@ -48568,7 +48568,7 @@
         <v>1</v>
       </c>
       <c r="BZ84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA84" s="1">
         <v>0</v>
@@ -49116,28 +49116,28 @@
         <v>1</v>
       </c>
       <c r="BP85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX85" s="1">
         <v>1</v>
@@ -49146,7 +49146,7 @@
         <v>1</v>
       </c>
       <c r="BZ85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA85" s="1">
         <v>0</v>
@@ -49694,28 +49694,28 @@
         <v>1</v>
       </c>
       <c r="BP86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX86" s="1">
         <v>1</v>
@@ -49724,7 +49724,7 @@
         <v>1</v>
       </c>
       <c r="BZ86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA86" s="1">
         <v>0</v>
@@ -50272,28 +50272,28 @@
         <v>1</v>
       </c>
       <c r="BP87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX87" s="1">
         <v>1</v>
@@ -50302,7 +50302,7 @@
         <v>1</v>
       </c>
       <c r="BZ87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA87" s="1">
         <v>0</v>
@@ -50850,28 +50850,28 @@
         <v>1</v>
       </c>
       <c r="BP88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX88" s="1">
         <v>1</v>
@@ -50880,7 +50880,7 @@
         <v>1</v>
       </c>
       <c r="BZ88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA88" s="1">
         <v>0</v>
@@ -51428,28 +51428,28 @@
         <v>1</v>
       </c>
       <c r="BP89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX89" s="1">
         <v>1</v>
@@ -51458,7 +51458,7 @@
         <v>1</v>
       </c>
       <c r="BZ89" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA89" s="1">
         <v>0</v>
@@ -52006,28 +52006,28 @@
         <v>1</v>
       </c>
       <c r="BP90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX90" s="1">
         <v>1</v>
@@ -52036,7 +52036,7 @@
         <v>1</v>
       </c>
       <c r="BZ90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA90" s="1">
         <v>0</v>
@@ -52584,28 +52584,28 @@
         <v>1</v>
       </c>
       <c r="BP91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX91" s="1">
         <v>1</v>
@@ -52614,7 +52614,7 @@
         <v>1</v>
       </c>
       <c r="BZ91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA91" s="1">
         <v>0</v>
@@ -53162,28 +53162,28 @@
         <v>1</v>
       </c>
       <c r="BP92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX92" s="1">
         <v>1</v>
@@ -91686,7 +91686,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A92:BY99 BZ93:CI99 BZ92:GJ92 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:GJ95 DB103:GJ126 DB97:EF102 EG96:GJ102 CJ96:EF96 A1:GJ91">
+  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:GJ95 DB103:GJ126 DB97:EF102 EG96:GJ102 CJ96:EF96 A1:GJ92">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -91698,7 +91698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A92:BY99 BZ93:CI99 BZ92:XFD92 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:XFD95 DB103:XFD126 DB97:EF102 EG96:XFD102 CJ96:EF96 A1:XFD91">
+  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:XFD95 DB103:XFD126 DB97:EF102 EG96:XFD102 CJ96:EF96 A1:XFD92">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Fixes for vehicles since restructuring
</commit_message>
<xml_diff>
--- a/assets/Meshes/Mesh_Inspection.xlsx
+++ b/assets/Meshes/Mesh_Inspection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\assets\Meshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D84257-CE61-48BF-BA5F-7D20F7F04049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA72093F-0B0A-4FCA-98B0-536F646E2C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,8 +351,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CE93" sqref="CE93"/>
+    <sheetView tabSelected="1" topLeftCell="I52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="CA65" sqref="BW65:CA83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28305,16 +28305,16 @@
         <v>1</v>
       </c>
       <c r="BO49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS49" s="1">
         <v>0</v>
@@ -28883,16 +28883,16 @@
         <v>1</v>
       </c>
       <c r="BO50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS50" s="1">
         <v>0</v>
@@ -29461,16 +29461,16 @@
         <v>1</v>
       </c>
       <c r="BO51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS51" s="1">
         <v>0</v>
@@ -30039,16 +30039,16 @@
         <v>1</v>
       </c>
       <c r="BO52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS52" s="1">
         <v>0</v>
@@ -30617,16 +30617,16 @@
         <v>1</v>
       </c>
       <c r="BO53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS53" s="1">
         <v>0</v>
@@ -31195,16 +31195,16 @@
         <v>1</v>
       </c>
       <c r="BO54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS54" s="1">
         <v>0</v>
@@ -31773,16 +31773,16 @@
         <v>1</v>
       </c>
       <c r="BO55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS55" s="1">
         <v>0</v>
@@ -32351,16 +32351,16 @@
         <v>1</v>
       </c>
       <c r="BO56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS56" s="1">
         <v>0</v>
@@ -32929,16 +32929,16 @@
         <v>1</v>
       </c>
       <c r="BO57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS57" s="1">
         <v>0</v>
@@ -33522,46 +33522,46 @@
         <v>1</v>
       </c>
       <c r="BT58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH58" s="1">
         <v>1</v>
@@ -34100,46 +34100,46 @@
         <v>1</v>
       </c>
       <c r="BT59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH59" s="1">
         <v>1</v>
@@ -34678,46 +34678,46 @@
         <v>1</v>
       </c>
       <c r="BT60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH60" s="1">
         <v>1</v>
@@ -49688,10 +49688,10 @@
         <v>1</v>
       </c>
       <c r="BN86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP86" s="1">
         <v>0</v>
@@ -50266,10 +50266,10 @@
         <v>1</v>
       </c>
       <c r="BN87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP87" s="1">
         <v>0</v>
@@ -50844,10 +50844,10 @@
         <v>1</v>
       </c>
       <c r="BN88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP88" s="1">
         <v>0</v>
@@ -51422,10 +51422,10 @@
         <v>1</v>
       </c>
       <c r="BN89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP89" s="1">
         <v>0</v>
@@ -52000,10 +52000,10 @@
         <v>1</v>
       </c>
       <c r="BN90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP90" s="1">
         <v>0</v>
@@ -52578,10 +52578,10 @@
         <v>1</v>
       </c>
       <c r="BN91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP91" s="1">
         <v>0</v>
@@ -53156,10 +53156,10 @@
         <v>1</v>
       </c>
       <c r="BN92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP92" s="1">
         <v>0</v>
@@ -57783,16 +57783,16 @@
         <v>1</v>
       </c>
       <c r="BO100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS100" s="1">
         <v>0</v>
@@ -58361,16 +58361,16 @@
         <v>1</v>
       </c>
       <c r="BO101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS101" s="1">
         <v>0</v>
@@ -58939,16 +58939,16 @@
         <v>1</v>
       </c>
       <c r="BO102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS102" s="1">
         <v>0</v>
@@ -59517,16 +59517,16 @@
         <v>1</v>
       </c>
       <c r="BO103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS103" s="1">
         <v>0</v>
@@ -60095,16 +60095,16 @@
         <v>1</v>
       </c>
       <c r="BO104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS104" s="1">
         <v>0</v>
@@ -60673,16 +60673,16 @@
         <v>1</v>
       </c>
       <c r="BO105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS105" s="1">
         <v>0</v>
@@ -61251,16 +61251,16 @@
         <v>1</v>
       </c>
       <c r="BO106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS106" s="1">
         <v>0</v>
@@ -61829,16 +61829,16 @@
         <v>1</v>
       </c>
       <c r="BO107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS107" s="1">
         <v>0</v>
@@ -62422,43 +62422,43 @@
         <v>1</v>
       </c>
       <c r="BT108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG108" s="1">
         <v>0</v>
@@ -63000,31 +63000,31 @@
         <v>1</v>
       </c>
       <c r="BT109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC109" s="1">
         <v>0</v>
@@ -63578,19 +63578,19 @@
         <v>1</v>
       </c>
       <c r="BT110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY110" s="1">
         <v>0</v>
@@ -91686,7 +91686,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:GJ95 DB103:GJ126 DB97:EF102 EG96:GJ102 CJ96:EF96 A1:GJ92">
+  <conditionalFormatting sqref="A158:GJ158 A124:BA157 BO127:GJ157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:GJ95 DB103:GJ126 DB97:EF102 EG96:GJ102 CJ96:EF96 A100:DA112 A1:GJ92">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -91698,7 +91698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A100:DA112 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:XFD95 DB103:XFD126 DB97:EF102 EG96:XFD102 CJ96:EF96 A1:XFD92">
+  <conditionalFormatting sqref="A158:XFD1048576 A124:BA157 BO127:XFD157 BO124:CY126 DA115:DA126 A123:CY123 CZ122:CZ126 A113:CA115 CB113:DA114 CB115:CZ115 CJ97:DA99 A93:CI99 A116:CZ119 CL120:CZ121 CL122:CY122 A120:CK122 CJ93:XFD95 DB103:XFD126 DB97:EF102 EG96:XFD102 CJ96:EF96 A100:DA112 A1:XFD92">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>